<commit_message>
planilha com conjunto 1
</commit_message>
<xml_diff>
--- a/data/resultado.xlsx
+++ b/data/resultado.xlsx
@@ -17,15 +17,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>somente matriz</t>
   </si>
   <si>
     <t>alfa = (1 - taxa de ratings)</t>
-  </si>
-  <si>
-    <t>taxa de trust</t>
   </si>
   <si>
     <t>alfa fixo 0.7</t>
@@ -128,16 +125,12 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -158,24 +151,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B20" activeCellId="0" pane="topLeft" sqref="B20"/>
+      <selection activeCell="B6" activeCellId="0" pane="topLeft" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.3"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5765306122449"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.4183673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.4234693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.9948979591837"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.4234693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.7142857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.9948979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.4234693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.7142857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -191,79 +183,76 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="s">
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
-      <c r="A3" s="0" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
+      <c r="A4" s="1" t="n">
+        <v>1.08304948340836</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>1.08273087819138</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1.08055252637603</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>1.0808622487661</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1.08066420628093</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
+      <c r="A6" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
-      <c r="A4" s="0" t="n">
-        <v>0.965455745168839</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>0.966028046104229</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>0.984742015179069</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>0.986357019990015</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>0.985748147629004</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
-      <c r="A6" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
       <c r="A7" s="0" t="n">
         <v>1.07414447099318</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1.07394817643996</v>
       </c>
+      <c r="C7" s="0" t="n">
+        <v>1.07117237335176</v>
+      </c>
       <c r="D7" s="0" t="n">
-        <v>1.07117237335176</v>
+        <v>1.07160836352875</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>1.07160836352875</v>
-      </c>
-      <c r="F7" s="0" t="n">
         <v>1.07134852007946</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="10">
       <c r="A10" s="0" t="n">
         <v>1.05975173991412</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1.05954729827638</v>
       </c>
+      <c r="C10" s="0" t="n">
+        <v>1.05713716175937</v>
+      </c>
       <c r="D10" s="0" t="n">
-        <v>1.05713716175937</v>
+        <v>1.05774097009947</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>1.05774097009947</v>
-      </c>
-      <c r="F10" s="0" t="n">
         <v>1.05738353340525</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="13">
@@ -273,26 +262,26 @@
       <c r="B13" s="0" t="n">
         <v>1.06178587465345</v>
       </c>
+      <c r="C13" s="1" t="n">
+        <v>1.05922070216772</v>
+      </c>
       <c r="D13" s="1" t="n">
-        <v>1.05922070216772</v>
-      </c>
-      <c r="E13" s="1" t="n">
         <v>1.0592747850318</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="E13" s="0" t="n">
         <v>1.05917647179964</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="14">
+      <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="15">
       <c r="A15" s="0" t="s">
-        <v>10</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="16">
       <c r="A16" s="0" t="n">
@@ -301,45 +290,45 @@
       <c r="B16" s="1" t="n">
         <v>1.05239879525754</v>
       </c>
+      <c r="C16" s="1" t="n">
+        <v>1.05068481691631</v>
+      </c>
       <c r="D16" s="1" t="n">
-        <v>1.05068481691631</v>
+        <v>1.05069213763927</v>
       </c>
       <c r="E16" s="1" t="n">
-        <v>1.05069213763927</v>
-      </c>
-      <c r="F16" s="1" t="n">
         <v>1.0506002364917</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="17">
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="19">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="20">
-      <c r="A20" s="2" t="n">
-        <f aca="false">AVERAGE(A7,A10,A13, A16)</f>
-        <v>1.06229964971168</v>
-      </c>
-      <c r="B20" s="2" t="n">
-        <f aca="false">AVERAGE(B7,B10,B13, B16)</f>
-        <v>1.06192003615683</v>
-      </c>
-      <c r="D20" s="2" t="n">
-        <f aca="false">AVERAGE(D7,D10,D13, D16)</f>
-        <v>1.05955376354879</v>
-      </c>
-      <c r="E20" s="2" t="n">
-        <f aca="false">AVERAGE(E7,E10,E13, E16)</f>
-        <v>1.05982906407482</v>
-      </c>
-      <c r="F20" s="2" t="n">
-        <f aca="false">AVERAGE(F7,F10,F13,F16)</f>
-        <v>1.05962719044401</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="20">
+      <c r="A20" s="0" t="n">
+        <f aca="false">AVERAGE(A4,A7,A10,A13, A16)</f>
+        <v>1.06644961645102</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <f aca="false">AVERAGE(B4,B7,B10,B13, B16)</f>
+        <v>1.06608220456374</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <f aca="false">AVERAGE(C4,C7,C10,C13, C16)</f>
+        <v>1.06375351611424</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <f aca="false">AVERAGE(D4,D7,D10,D13, D16)</f>
+        <v>1.06403570101308</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <f aca="false">AVERAGE(E4,E7,E10,E13,E16)</f>
+        <v>1.0638345936114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>